<commit_message>
Finish Zindi, Update Adult, Compass
1. Create the biased model for Zinid
2. Fix the error when test with Adult, Compass
3. Set up for german but we do not use this dataset for this time.
</commit_message>
<xml_diff>
--- a/Experiment Result.xlsx
+++ b/Experiment Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuhr\OneDrive\桌面\AuFair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8F8431-FA0D-46F4-A4A7-064A2A6F8333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D894236-ABC1-4CDF-B2F4-CC6507D60022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="588" yWindow="3636" windowWidth="20808" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="20808" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="17">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,23 +82,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Bank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>German</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>recidivism</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>law</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -110,11 +94,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>metric optimized become worse</t>
+    <t>EOP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">shuffle=True, only 8 samples </t>
+    <t>H0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,25 +125,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,10 +146,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -454,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -479,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -511,10 +485,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.22309999999999999</v>
+        <v>0.256885703570982</v>
       </c>
       <c r="G2">
-        <v>2.6859999999999998E-2</v>
+        <v>4.9285845083318097E-2</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -534,10 +508,10 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>0.23130000000000001</v>
+        <v>0.22696779032459599</v>
       </c>
       <c r="G3">
-        <v>1.468E-2</v>
+        <v>4.4753054124048501E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -557,10 +531,10 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <v>0.23930000000000001</v>
+        <v>0.21696737364056801</v>
       </c>
       <c r="G4">
-        <v>4.6449999999999998E-2</v>
+        <v>3.9223585423914999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -580,10 +554,10 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>0.2331</v>
+        <v>0.22317596566523601</v>
       </c>
       <c r="G5">
-        <v>2.494E-2</v>
+        <v>4.8689408010045197E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -603,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>0.23630000000000001</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9.8160000000000001E-4</v>
+        <v>0.21550897954081399</v>
+      </c>
+      <c r="G6">
+        <v>4.9205404556988498E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -626,10 +600,10 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0.23130000000000001</v>
+        <v>0.22546242292951099</v>
       </c>
       <c r="G7">
-        <v>3.635E-2</v>
+        <v>5.1731823883722702E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -649,10 +623,10 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>0.248</v>
+        <v>0.239166666666666</v>
       </c>
       <c r="G8">
-        <v>4.7440000000000003E-2</v>
+        <v>4.41508377127229E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -672,10 +646,10 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>0.22320000000000001</v>
+        <v>0.22716666666666599</v>
       </c>
       <c r="G9">
-        <v>1.0829999999999999E-2</v>
+        <v>3.17864954601965E-3</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -695,10 +669,10 @@
         <v>4</v>
       </c>
       <c r="F10">
-        <v>0.2288</v>
+        <v>0.22216666666666601</v>
       </c>
       <c r="G10">
-        <v>4.1360000000000001E-2</v>
+        <v>4.2997542997542902E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -718,10 +692,10 @@
         <v>5</v>
       </c>
       <c r="F11">
-        <v>0.22770000000000001</v>
+        <v>0.23303883980663401</v>
       </c>
       <c r="G11">
-        <v>6.8110000000000004E-2</v>
+        <v>5.5654325097214401E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -732,13 +706,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.44678111587982799</v>
+      </c>
+      <c r="G12">
+        <v>0.119421906693712</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -749,7 +729,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -757,6 +737,12 @@
       <c r="E13">
         <v>2</v>
       </c>
+      <c r="F13">
+        <v>0.53155860884499695</v>
+      </c>
+      <c r="G13">
+        <v>5.11152416356878E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -766,7 +752,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -774,6 +760,12 @@
       <c r="E14">
         <v>3</v>
       </c>
+      <c r="F14">
+        <v>0.56462000858737604</v>
+      </c>
+      <c r="G14">
+        <v>4.2746327776860799E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -783,7 +775,7 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -791,6 +783,12 @@
       <c r="E15">
         <v>4</v>
       </c>
+      <c r="F15">
+        <v>0.47702876771146402</v>
+      </c>
+      <c r="G15">
+        <v>6.8336761680869704E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -800,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -808,13 +806,19 @@
       <c r="E16">
         <v>5</v>
       </c>
+      <c r="F16">
+        <v>0.55756013745704402</v>
+      </c>
+      <c r="G16">
+        <v>3.68550368550368E-3</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -824,6 +828,12 @@
       </c>
       <c r="E17">
         <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.18537414965986301</v>
+      </c>
+      <c r="G17">
+        <v>5.0778543558326797E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -831,7 +841,7 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -842,14 +852,19 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="F18">
+        <v>0.23315621679064799</v>
+      </c>
+      <c r="G18">
+        <v>5.63029124085591E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -860,14 +875,19 @@
       <c r="E19">
         <v>3</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="F19">
+        <v>0.26163655685441001</v>
+      </c>
+      <c r="G19">
+        <v>4.9473342126894901E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -878,13 +898,19 @@
       <c r="E20">
         <v>4</v>
       </c>
+      <c r="F20">
+        <v>0.157279489904357</v>
+      </c>
+      <c r="G20">
+        <v>9.5068235105508797E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -895,28 +921,34 @@
       <c r="E21">
         <v>5</v>
       </c>
+      <c r="F21">
+        <v>0.22019128586609901</v>
+      </c>
+      <c r="G21">
+        <v>7.8303411894835306E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0.38500000000000001</v>
+        <v>0.256885703570982</v>
       </c>
       <c r="G22">
-        <v>4.9589999999999999E-3</v>
+        <v>4.9285845083318097E-2</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -924,22 +956,22 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3.4290000000000001E-2</v>
+        <v>0.25530230426267703</v>
+      </c>
+      <c r="G23">
+        <v>3.6281947314725102E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -947,22 +979,22 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E24">
         <v>3</v>
       </c>
       <c r="F24">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0.19370000000000001</v>
+        <v>0.26546939455810598</v>
+      </c>
+      <c r="G24">
+        <v>1.3557171632615399E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -970,22 +1002,22 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="F25">
-        <v>0.3</v>
+        <v>0.255177299054127</v>
       </c>
       <c r="G25">
-        <v>5.4429999999999999E-2</v>
+        <v>4.7088445339681297E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -993,22 +1025,22 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E26">
         <v>5</v>
       </c>
       <c r="F26">
-        <v>0.28499999999999998</v>
+        <v>0.25767740322513399</v>
       </c>
       <c r="G26">
-        <v>5.9420000000000001E-2</v>
+        <v>3.5183247442906698E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1016,22 +1048,22 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
         <v>8</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0.48880000000000001</v>
+        <v>0.22546242292951099</v>
       </c>
       <c r="G27">
-        <v>0.1053</v>
+        <v>5.1731823883722702E-3</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1039,22 +1071,22 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
         <v>8</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28">
-        <v>0.1053</v>
+        <v>0.222</v>
       </c>
       <c r="G28">
-        <v>0.1799</v>
+        <v>0.142287606464473</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1062,22 +1094,22 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
         <v>8</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
       <c r="F29">
-        <v>0.55169999999999997</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="G29">
-        <v>4.922E-2</v>
+        <v>0.11260602055107</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1085,22 +1117,22 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E30">
         <v>4</v>
       </c>
       <c r="F30">
-        <v>0.4526</v>
+        <v>0.22216666666666601</v>
       </c>
       <c r="G30">
-        <v>0.1042</v>
+        <v>4.2997542997542902E-2</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1108,22 +1140,22 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E31">
         <v>5</v>
       </c>
       <c r="F31">
-        <v>0.51029999999999998</v>
+        <v>0.23303883980663401</v>
       </c>
       <c r="G31">
-        <v>2.426E-2</v>
+        <v>5.5654325097214401E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1131,16 +1163,22 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E32">
         <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0.28454935622317501</v>
+      </c>
+      <c r="G32">
+        <v>0.161806964164976</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1148,84 +1186,114 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
+      <c r="F33">
+        <v>0.58995276942893904</v>
+      </c>
+      <c r="G33">
+        <v>3.5974287484510502E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
+      <c r="F34">
+        <v>0.59682267067410899</v>
+      </c>
+      <c r="G34">
+        <v>3.6276613302525101E-2</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
+      <c r="F35">
+        <v>0.58866466294547004</v>
+      </c>
+      <c r="G35">
+        <v>8.3896561857185192E-3</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E36">
         <v>5</v>
       </c>
+      <c r="F36">
+        <v>0.38187285223367601</v>
+      </c>
+      <c r="G36">
+        <v>1.5970515970515901E-2</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E37">
         <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0.23278061224489699</v>
+      </c>
+      <c r="G37">
+        <v>5.9366225431207398E-2</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1233,68 +1301,92 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E38">
         <v>2</v>
       </c>
+      <c r="F38">
+        <v>0.23315621679064799</v>
+      </c>
+      <c r="G38">
+        <v>5.63029124085591E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E39">
         <v>3</v>
       </c>
+      <c r="F39">
+        <v>0.26163655685441001</v>
+      </c>
+      <c r="G39">
+        <v>4.9473342126894901E-2</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E40">
         <v>4</v>
       </c>
+      <c r="F40">
+        <v>0.14303931987247601</v>
+      </c>
+      <c r="G40">
+        <v>5.6511893549227497E-2</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
+      <c r="F41">
+        <v>0.212539851222104</v>
+      </c>
+      <c r="G41">
+        <v>6.5089764315493903E-2</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
@@ -1307,16 +1399,16 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42">
-        <v>0.2485</v>
+        <v>0.32780532522188399</v>
       </c>
       <c r="G42">
-        <v>6.4399999999999999E-2</v>
+        <v>4.26831820441049E-2</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1330,16 +1422,16 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
       <c r="F43">
-        <v>0.23369999999999999</v>
+        <v>0.16617359056627301</v>
       </c>
       <c r="G43">
-        <v>1.8890000000000001E-2</v>
+        <v>0.176994009469746</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1353,16 +1445,16 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E44">
         <v>3</v>
       </c>
       <c r="F44">
-        <v>0.23960000000000001</v>
+        <v>0.32693028876203101</v>
       </c>
       <c r="G44">
-        <v>5.076E-2</v>
+        <v>4.42403275171998E-2</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1376,16 +1468,16 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E45">
         <v>4</v>
       </c>
       <c r="F45">
-        <v>0.2281</v>
+        <v>0.164590191257969</v>
       </c>
       <c r="G45">
-        <v>8.1350000000000006E-2</v>
+        <v>0.18908232401182401</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1399,16 +1491,16 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E46">
         <v>5</v>
       </c>
       <c r="F46">
-        <v>0.23280000000000001</v>
+        <v>0.32713863077628202</v>
       </c>
       <c r="G46">
-        <v>6.3210000000000002E-2</v>
+        <v>4.0668898945771297E-2</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1422,16 +1514,16 @@
         <v>8</v>
       </c>
       <c r="D47">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
-        <v>0.23130000000000001</v>
+        <v>0.17430428261956299</v>
       </c>
       <c r="G47">
-        <v>3.3770000000000001E-2</v>
+        <v>0.140951077659938</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1445,16 +1537,16 @@
         <v>8</v>
       </c>
       <c r="D48">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E48">
         <v>2</v>
       </c>
       <c r="F48">
-        <v>0.2198</v>
+        <v>0.266166666666666</v>
       </c>
       <c r="G48">
-        <v>1.7239999999999998E-2</v>
+        <v>3.9134445890512501E-2</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1468,16 +1560,16 @@
         <v>8</v>
       </c>
       <c r="D49">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E49">
         <v>3</v>
       </c>
       <c r="F49">
-        <v>0.21820000000000001</v>
+        <v>0.19950000000000001</v>
       </c>
       <c r="G49">
-        <v>1.089E-2</v>
+        <v>5.8281798297376702E-2</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1491,16 +1583,16 @@
         <v>8</v>
       </c>
       <c r="D50">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50">
-        <v>0.2147</v>
+        <v>0.19466666666666599</v>
       </c>
       <c r="G50">
-        <v>2.826E-2</v>
+        <v>5.3235053235053398E-3</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1514,16 +1606,16 @@
         <v>8</v>
       </c>
       <c r="D51">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E51">
         <v>5</v>
       </c>
       <c r="F51">
-        <v>0.2387</v>
+        <v>0.195865977662943</v>
       </c>
       <c r="G51">
-        <v>8.183E-2</v>
+        <v>3.7066317652933098E-2</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1534,13 +1626,19 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E52">
         <v>1</v>
+      </c>
+      <c r="F52">
+        <v>0.342060085836909</v>
+      </c>
+      <c r="G52">
+        <v>9.0348208248816703E-2</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1551,14 +1649,20 @@
         <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D53">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E53">
         <v>2</v>
       </c>
+      <c r="F53">
+        <v>0.26019750966079802</v>
+      </c>
+      <c r="G53">
+        <v>0.20546778190830201</v>
+      </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
@@ -1568,14 +1672,20 @@
         <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D54">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
+      <c r="F54">
+        <v>0.441820523829969</v>
+      </c>
+      <c r="G54">
+        <v>7.5540518237332793E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
@@ -1585,14 +1695,20 @@
         <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D55">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E55">
         <v>4</v>
       </c>
+      <c r="F55">
+        <v>0.44010304851867699</v>
+      </c>
+      <c r="G55">
+        <v>8.2530120481927594E-2</v>
+      </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
@@ -1602,30 +1718,42 @@
         <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D56">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E56">
         <v>5</v>
       </c>
+      <c r="F56">
+        <v>0.39046391752577297</v>
+      </c>
+      <c r="G56">
+        <v>6.5110565110565094E-2</v>
+      </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E57">
         <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0.18537414965986301</v>
+      </c>
+      <c r="G57">
+        <v>5.0778543558326797E-2</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1633,190 +1761,214 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
       </c>
       <c r="D58">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E58">
         <v>2</v>
       </c>
+      <c r="F58">
+        <v>0.48714133900106199</v>
+      </c>
+      <c r="G58">
+        <v>7.5910755545814002E-2</v>
+      </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
       <c r="D59">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E59">
         <v>3</v>
       </c>
+      <c r="F59">
+        <v>0.65674814027630102</v>
+      </c>
+      <c r="G59">
+        <v>3.3472883332377502E-2</v>
+      </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E60">
         <v>4</v>
       </c>
+      <c r="F60">
+        <v>0.41721572794898998</v>
+      </c>
+      <c r="G60">
+        <v>0.20398388809843401</v>
+      </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
       <c r="D61">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E61">
         <v>5</v>
       </c>
+      <c r="F61">
+        <v>0.441232731137088</v>
+      </c>
+      <c r="G61">
+        <v>9.0802348336594896E-2</v>
+      </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D62">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62">
-        <v>0.36499999999999999</v>
+        <v>0.136692176870748</v>
       </c>
       <c r="G62">
-        <v>6.8430000000000005E-2</v>
+        <v>3.2044269408890297E-2</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E63">
         <v>2</v>
       </c>
       <c r="F63">
-        <v>0.29499999999999998</v>
+        <v>0.12731137088204</v>
       </c>
       <c r="G63">
-        <v>0.23519999999999999</v>
+        <v>6.4905887832543294E-2</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D64">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E64">
         <v>3</v>
       </c>
       <c r="F64">
-        <v>0.30499999999999999</v>
+        <v>0.12327311370882001</v>
       </c>
       <c r="G64">
-        <v>0.1903</v>
+        <v>3.7907897000630797E-2</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D65">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E65">
         <v>4</v>
       </c>
       <c r="F65">
-        <v>0.28499999999999998</v>
+        <v>0.12433581296493</v>
       </c>
       <c r="G65">
-        <v>0.1012</v>
+        <v>6.23234003326586E-3</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D66">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E66">
         <v>5</v>
       </c>
       <c r="F66">
-        <v>0.31</v>
+        <v>0.12986184909670501</v>
       </c>
       <c r="G66">
-        <v>0.1125</v>
+        <v>1.09078533140474E-2</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
@@ -1828,18 +1980,18 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>0.29399999999999998</v>
+        <v>0.13584183673469299</v>
       </c>
       <c r="G67">
-        <v>0.1641</v>
+        <v>5.9822047186668101E-2</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B68" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
@@ -1851,18 +2003,18 @@
         <v>2</v>
       </c>
       <c r="F68">
-        <v>0.58779999999999999</v>
+        <v>0.12624867162592901</v>
       </c>
       <c r="G68">
-        <v>5.9630000000000004E-3</v>
+        <v>3.5115117309149999E-2</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -1874,18 +2026,18 @@
         <v>3</v>
       </c>
       <c r="F69">
-        <v>0.58609999999999995</v>
+        <v>0.121572794899043</v>
       </c>
       <c r="G69">
-        <v>2.664E-2</v>
+        <v>2.3436753264131801E-2</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
         <v>8</v>
@@ -1897,18 +2049,18 @@
         <v>4</v>
       </c>
       <c r="F70">
-        <v>0.53239999999999998</v>
+        <v>0.125611052072263</v>
       </c>
       <c r="G70">
-        <v>7.5649999999999995E-2</v>
+        <v>4.5229554517945497E-2</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
         <v>8</v>
@@ -1920,995 +2072,355 @@
         <v>5</v>
       </c>
       <c r="F71">
-        <v>0.56310000000000004</v>
+        <v>0.130924548352816</v>
       </c>
       <c r="G71">
-        <v>2.9479999999999999E-2</v>
+        <v>1.6489406959925099E-2</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D72">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E72">
         <v>1</v>
+      </c>
+      <c r="F72">
+        <v>0.13350340136054401</v>
+      </c>
+      <c r="G72">
+        <v>0.16122415490646499</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B73" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D73">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E73">
         <v>2</v>
       </c>
+      <c r="F73">
+        <v>0.121572794899043</v>
+      </c>
+      <c r="G73">
+        <v>1.6685388640784601E-2</v>
+      </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D74">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E74">
         <v>3</v>
       </c>
+      <c r="F74">
+        <v>0.79808714133900105</v>
+      </c>
+      <c r="G74">
+        <v>0.17885339603525</v>
+      </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D75">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E75">
         <v>4</v>
       </c>
+      <c r="F75">
+        <v>0.131774707757704</v>
+      </c>
+      <c r="G75">
+        <v>5.9347508065970597E-2</v>
+      </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B76" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D76">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="E76">
         <v>5</v>
       </c>
+      <c r="F76">
+        <v>0.130074388947927</v>
+      </c>
+      <c r="G76">
+        <v>0.13676508125584899</v>
+      </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
       </c>
       <c r="D77">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E77">
         <v>1</v>
+      </c>
+      <c r="F77">
+        <v>0.13371598639455701</v>
+      </c>
+      <c r="G77">
+        <v>3.4569521934142797E-2</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C78" t="s">
         <v>8</v>
       </c>
       <c r="D78">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E78">
         <v>2</v>
       </c>
+      <c r="F78">
+        <v>0.1192348565356</v>
+      </c>
+      <c r="G78">
+        <v>3.7334356192406999E-2</v>
+      </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
       </c>
       <c r="D79">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>3</v>
       </c>
+      <c r="F79">
+        <v>0.1192348565356</v>
+      </c>
+      <c r="G79">
+        <v>5.12416126627286E-2</v>
+      </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C80" t="s">
         <v>8</v>
       </c>
       <c r="D80">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="F80">
+        <v>0.12199787460148701</v>
+      </c>
+      <c r="G80">
+        <v>6.6130939259734201E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
       </c>
       <c r="D81">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="F81">
+        <v>0.12199787460148701</v>
+      </c>
+      <c r="G81">
+        <v>4.1776567684846298E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D82">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>1</v>
       </c>
       <c r="F82">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="G82" s="1">
-        <v>0.1628</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+        <v>0.12733843537414899</v>
+      </c>
+      <c r="G82">
+        <v>1.68198227765014E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D83">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E83">
         <v>2</v>
       </c>
       <c r="F83">
-        <v>0.31080000000000002</v>
+        <v>0.1192348565356</v>
       </c>
       <c r="G83">
-        <v>1.567E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+        <v>1.73886042539977E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D84">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <v>3</v>
       </c>
       <c r="F84">
-        <v>0.33350000000000002</v>
+        <v>1.73886042539977E-2</v>
       </c>
       <c r="G84">
-        <v>1.6469999999999999E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>0.11753453772582299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D85">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>4</v>
       </c>
       <c r="F85">
-        <v>0.31780000000000003</v>
+        <v>0.116471838469713</v>
       </c>
       <c r="G85">
-        <v>1.272E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>1.7234123564658001E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D86">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="E86">
         <v>5</v>
       </c>
       <c r="F86">
-        <v>0.33029999999999998</v>
+        <v>0.122635494155154</v>
       </c>
       <c r="G86">
-        <v>5.3920000000000001E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" t="s">
-        <v>6</v>
-      </c>
-      <c r="B87" t="s">
-        <v>7</v>
-      </c>
-      <c r="C87" t="s">
-        <v>8</v>
-      </c>
-      <c r="D87">
-        <v>0.01</v>
-      </c>
-      <c r="E87">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>0.1883</v>
-      </c>
-      <c r="G87">
-        <v>5.049E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" t="s">
-        <v>6</v>
-      </c>
-      <c r="B88" t="s">
-        <v>7</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
-      </c>
-      <c r="D88">
-        <v>0.01</v>
-      </c>
-      <c r="E88">
-        <v>2</v>
-      </c>
-      <c r="F88">
-        <v>0.26779999999999998</v>
-      </c>
-      <c r="G88">
-        <v>3.585E-2</v>
-      </c>
-      <c r="H88" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>8</v>
-      </c>
-      <c r="D89">
-        <v>0.01</v>
-      </c>
-      <c r="E89">
-        <v>3</v>
-      </c>
-      <c r="F89">
-        <v>0.26729999999999998</v>
-      </c>
-      <c r="G89">
-        <v>5.7880000000000001E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" t="s">
-        <v>7</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90">
-        <v>0.01</v>
-      </c>
-      <c r="E90">
-        <v>4</v>
-      </c>
-      <c r="F90">
-        <v>0.19919999999999999</v>
-      </c>
-      <c r="G90">
-        <v>2.0480000000000002E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>6</v>
-      </c>
-      <c r="B91" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D91">
-        <v>0.01</v>
-      </c>
-      <c r="E91">
-        <v>5</v>
-      </c>
-      <c r="F91">
-        <v>0.19439999999999999</v>
-      </c>
-      <c r="G91" s="1">
-        <v>9.5319999999999997E-4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" t="s">
-        <v>11</v>
-      </c>
-      <c r="C92" t="s">
-        <v>12</v>
-      </c>
-      <c r="D92">
-        <v>0.01</v>
-      </c>
-      <c r="E92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93">
-        <v>0.01</v>
-      </c>
-      <c r="E93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
-        <v>6</v>
-      </c>
-      <c r="B94" t="s">
-        <v>11</v>
-      </c>
-      <c r="C94" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94">
-        <v>0.01</v>
-      </c>
-      <c r="E94">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" t="s">
-        <v>6</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
-      </c>
-      <c r="C95" t="s">
-        <v>12</v>
-      </c>
-      <c r="D95">
-        <v>0.01</v>
-      </c>
-      <c r="E95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" t="s">
-        <v>6</v>
-      </c>
-      <c r="B96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C96" t="s">
-        <v>12</v>
-      </c>
-      <c r="D96">
-        <v>0.01</v>
-      </c>
-      <c r="E96">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" t="s">
-        <v>6</v>
-      </c>
-      <c r="B97" t="s">
-        <v>13</v>
-      </c>
-      <c r="C97" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97">
-        <v>0.01</v>
-      </c>
-      <c r="E97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
-      <c r="A98" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" t="s">
-        <v>13</v>
-      </c>
-      <c r="C98" t="s">
-        <v>8</v>
-      </c>
-      <c r="D98">
-        <v>0.01</v>
-      </c>
-      <c r="E98">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="A99" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99" t="s">
-        <v>13</v>
-      </c>
-      <c r="C99" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99">
-        <v>0.01</v>
-      </c>
-      <c r="E99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
-      <c r="A100" t="s">
-        <v>6</v>
-      </c>
-      <c r="B100" t="s">
-        <v>13</v>
-      </c>
-      <c r="C100" t="s">
-        <v>8</v>
-      </c>
-      <c r="D100">
-        <v>0.01</v>
-      </c>
-      <c r="E100">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
-      <c r="A101" t="s">
-        <v>6</v>
-      </c>
-      <c r="B101" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" t="s">
-        <v>8</v>
-      </c>
-      <c r="D101">
-        <v>0.01</v>
-      </c>
-      <c r="E101">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
-      <c r="A102" t="s">
-        <v>6</v>
-      </c>
-      <c r="B102" t="s">
-        <v>13</v>
-      </c>
-      <c r="C102" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102">
-        <v>0.01</v>
-      </c>
-      <c r="E102">
-        <v>1</v>
-      </c>
-      <c r="F102">
-        <v>0.23</v>
-      </c>
-      <c r="G102">
-        <v>8.2640000000000005E-2</v>
-      </c>
-      <c r="H102" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
-      <c r="A103" t="s">
-        <v>6</v>
-      </c>
-      <c r="B103" t="s">
-        <v>13</v>
-      </c>
-      <c r="C103" t="s">
-        <v>12</v>
-      </c>
-      <c r="D103">
-        <v>0.01</v>
-      </c>
-      <c r="E103">
-        <v>2</v>
-      </c>
-      <c r="F103">
-        <v>0.32</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" t="s">
-        <v>6</v>
-      </c>
-      <c r="B104" t="s">
-        <v>13</v>
-      </c>
-      <c r="C104" t="s">
-        <v>12</v>
-      </c>
-      <c r="D104">
-        <v>0.01</v>
-      </c>
-      <c r="E104">
-        <v>3</v>
-      </c>
-      <c r="F104">
-        <v>0.31</v>
-      </c>
-      <c r="G104">
-        <v>1.983E-2</v>
-      </c>
-      <c r="H104" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
-      <c r="A105" t="s">
-        <v>6</v>
-      </c>
-      <c r="B105" t="s">
-        <v>13</v>
-      </c>
-      <c r="C105" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105">
-        <v>0.01</v>
-      </c>
-      <c r="E105">
-        <v>4</v>
-      </c>
-      <c r="F105">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="G105">
-        <v>8.5019999999999998E-2</v>
-      </c>
-      <c r="H105" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="A106" t="s">
-        <v>6</v>
-      </c>
-      <c r="B106" t="s">
-        <v>13</v>
-      </c>
-      <c r="C106" t="s">
-        <v>12</v>
-      </c>
-      <c r="D106">
-        <v>0.01</v>
-      </c>
-      <c r="E106">
-        <v>5</v>
-      </c>
-      <c r="F106">
-        <v>0.41</v>
-      </c>
-      <c r="G106">
-        <v>0.51329999999999998</v>
-      </c>
-      <c r="H106" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8">
-      <c r="A107" t="s">
-        <v>6</v>
-      </c>
-      <c r="B107" t="s">
-        <v>14</v>
-      </c>
-      <c r="C107" t="s">
-        <v>8</v>
-      </c>
-      <c r="D107">
-        <v>0.01</v>
-      </c>
-      <c r="E107">
-        <v>1</v>
-      </c>
-      <c r="F107">
-        <v>0.4798</v>
-      </c>
-      <c r="G107">
-        <v>0.6855</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8">
-      <c r="A108" t="s">
-        <v>6</v>
-      </c>
-      <c r="B108" t="s">
-        <v>14</v>
-      </c>
-      <c r="C108" t="s">
-        <v>8</v>
-      </c>
-      <c r="D108">
-        <v>0.01</v>
-      </c>
-      <c r="E108">
-        <v>2</v>
-      </c>
-      <c r="F108">
-        <v>0.56889999999999996</v>
-      </c>
-      <c r="G108">
-        <v>0.1457</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8">
-      <c r="A109" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" t="s">
-        <v>14</v>
-      </c>
-      <c r="C109" t="s">
-        <v>8</v>
-      </c>
-      <c r="D109">
-        <v>0.01</v>
-      </c>
-      <c r="E109">
-        <v>3</v>
-      </c>
-      <c r="F109">
-        <v>0.40579999999999999</v>
-      </c>
-      <c r="G109">
-        <v>0.47070000000000001</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8">
-      <c r="A110" t="s">
-        <v>6</v>
-      </c>
-      <c r="B110" t="s">
-        <v>14</v>
-      </c>
-      <c r="C110" t="s">
-        <v>8</v>
-      </c>
-      <c r="D110">
-        <v>0.01</v>
-      </c>
-      <c r="E110">
-        <v>4</v>
-      </c>
-      <c r="F110">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="G110">
-        <v>0.2137</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8">
-      <c r="A111" t="s">
-        <v>6</v>
-      </c>
-      <c r="B111" t="s">
-        <v>14</v>
-      </c>
-      <c r="C111" t="s">
-        <v>8</v>
-      </c>
-      <c r="D111">
-        <v>0.01</v>
-      </c>
-      <c r="E111">
-        <v>5</v>
-      </c>
-      <c r="F111">
-        <v>0.24229999999999999</v>
-      </c>
-      <c r="G111">
-        <v>0.37009999999999998</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" t="s">
-        <v>6</v>
-      </c>
-      <c r="B112" t="s">
-        <v>15</v>
-      </c>
-      <c r="C112" t="s">
-        <v>10</v>
-      </c>
-      <c r="D112">
-        <v>0.01</v>
-      </c>
-      <c r="E112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
-      <c r="A113" t="s">
-        <v>6</v>
-      </c>
-      <c r="B113" t="s">
-        <v>15</v>
-      </c>
-      <c r="C113" t="s">
-        <v>10</v>
-      </c>
-      <c r="D113">
-        <v>0.01</v>
-      </c>
-      <c r="E113">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
-      <c r="A114" t="s">
-        <v>6</v>
-      </c>
-      <c r="B114" t="s">
-        <v>15</v>
-      </c>
-      <c r="C114" t="s">
-        <v>10</v>
-      </c>
-      <c r="D114">
-        <v>0.01</v>
-      </c>
-      <c r="E114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
-      <c r="A115" t="s">
-        <v>6</v>
-      </c>
-      <c r="B115" t="s">
-        <v>15</v>
-      </c>
-      <c r="C115" t="s">
-        <v>10</v>
-      </c>
-      <c r="D115">
-        <v>0.01</v>
-      </c>
-      <c r="E115">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
-      <c r="A116" t="s">
-        <v>6</v>
-      </c>
-      <c r="B116" t="s">
-        <v>15</v>
-      </c>
-      <c r="C116" t="s">
-        <v>10</v>
-      </c>
-      <c r="D116">
-        <v>0.01</v>
-      </c>
-      <c r="E116">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
-      <c r="A117" t="s">
-        <v>6</v>
-      </c>
-      <c r="B117" t="s">
-        <v>16</v>
-      </c>
-      <c r="C117" t="s">
-        <v>8</v>
-      </c>
-      <c r="D117">
-        <v>0.01</v>
-      </c>
-      <c r="E117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
-      <c r="A118" t="s">
-        <v>6</v>
-      </c>
-      <c r="B118" t="s">
-        <v>16</v>
-      </c>
-      <c r="C118" t="s">
-        <v>8</v>
-      </c>
-      <c r="D118">
-        <v>0.01</v>
-      </c>
-      <c r="E118">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
-      <c r="A119" t="s">
-        <v>6</v>
-      </c>
-      <c r="B119" t="s">
-        <v>16</v>
-      </c>
-      <c r="C119" t="s">
-        <v>8</v>
-      </c>
-      <c r="D119">
-        <v>0.01</v>
-      </c>
-      <c r="E119">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" t="s">
-        <v>6</v>
-      </c>
-      <c r="B120" t="s">
-        <v>16</v>
-      </c>
-      <c r="C120" t="s">
-        <v>8</v>
-      </c>
-      <c r="D120">
-        <v>0.01</v>
-      </c>
-      <c r="E120">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" t="s">
-        <v>6</v>
-      </c>
-      <c r="B121" t="s">
-        <v>16</v>
-      </c>
-      <c r="C121" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121">
-        <v>0.01</v>
-      </c>
-      <c r="E121">
-        <v>5</v>
+        <v>1.8752658895601099E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Compas + Bank
1. Compas should use 0 as favorable label
Thus, I flip the label
2. Bank was wrong about H0 H1, now fixed
</commit_message>
<xml_diff>
--- a/Experiment Result.xlsx
+++ b/Experiment Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuhr\OneDrive\桌面\AuFair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5E4EFB-934C-4E93-8D3F-A9E95C145783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DBC18C-D77D-4831-9229-7E5A29828645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="804" windowWidth="20808" windowHeight="11448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="21">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,15 +119,6 @@
   </si>
   <si>
     <t>Shuffle = True</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.07163323782183645  这两个TPR 也太低了吧？
-0.015873015870496346</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -456,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G130" sqref="G130"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -743,10 +734,10 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0.44678111587982799</v>
+        <v>0.25836909871244601</v>
       </c>
       <c r="G12">
-        <v>0.119421906693712</v>
+        <v>3.2170624636378098E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -766,10 +757,10 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0.53155860884499695</v>
+        <v>0.25418634607127499</v>
       </c>
       <c r="G13">
-        <v>5.11152416356878E-2</v>
+        <v>0.109763730245658</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -789,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>0.56462000858737604</v>
+        <v>0.34864748819235702</v>
       </c>
       <c r="G14">
-        <v>4.2746327776860799E-2</v>
+        <v>7.4488757286944596E-3</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -812,10 +803,10 @@
         <v>4</v>
       </c>
       <c r="F15">
-        <v>0.47702876771146402</v>
+        <v>0.28553027050236102</v>
       </c>
       <c r="G15">
-        <v>6.8336761680869704E-2</v>
+        <v>2.7571591588328E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -835,10 +826,10 @@
         <v>5</v>
       </c>
       <c r="F16">
-        <v>0.55756013745704402</v>
+        <v>0.231958762886597</v>
       </c>
       <c r="G16">
-        <v>3.68550368550368E-3</v>
+        <v>1.0440456769983701E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1203,10 +1194,10 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.28454935622317501</v>
+        <v>0.31158798283261802</v>
       </c>
       <c r="G32">
-        <v>0.161806964164976</v>
+        <v>2.86269635584703E-2</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1226,10 +1217,10 @@
         <v>2</v>
       </c>
       <c r="F33">
-        <v>0.58995276942893904</v>
+        <v>0.24645770717045901</v>
       </c>
       <c r="G33">
-        <v>3.5974287484510502E-2</v>
+        <v>0.11287357221092099</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1249,10 +1240,10 @@
         <v>3</v>
       </c>
       <c r="F34">
-        <v>0.59682267067410899</v>
+        <v>0.389437526835551</v>
       </c>
       <c r="G34">
-        <v>3.6276613302525101E-2</v>
+        <v>4.5942444711760899E-2</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1272,10 +1263,10 @@
         <v>4</v>
       </c>
       <c r="F35">
-        <v>0.58866466294547004</v>
+        <v>0.30356376127093099</v>
       </c>
       <c r="G35">
-        <v>8.3896561857185192E-3</v>
+        <v>2.2749913963303E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1295,10 +1286,10 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>0.38187285223367601</v>
+        <v>0.231958762886597</v>
       </c>
       <c r="G36">
-        <v>1.5970515970515901E-2</v>
+        <v>1.0440456769983701E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1663,10 +1654,10 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>0.342060085836909</v>
+        <v>0.30515021459227398</v>
       </c>
       <c r="G52">
-        <v>9.0348208248816703E-2</v>
+        <v>0.12232242026762501</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1686,10 +1677,10 @@
         <v>2</v>
       </c>
       <c r="F53">
-        <v>0.26019750966079802</v>
+        <v>0.250322026620867</v>
       </c>
       <c r="G53">
-        <v>0.20546778190830201</v>
+        <v>2.9494601783758401E-2</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1709,10 +1700,10 @@
         <v>3</v>
       </c>
       <c r="F54">
-        <v>0.441820523829969</v>
+        <v>0.35294117647058798</v>
       </c>
       <c r="G54">
-        <v>7.5540518237332793E-2</v>
+        <v>0.37007649363067102</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1732,10 +1723,10 @@
         <v>4</v>
       </c>
       <c r="F55">
-        <v>0.44010304851867699</v>
+        <v>0.27737226277372201</v>
       </c>
       <c r="G55">
-        <v>8.2530120481927594E-2</v>
+        <v>5.9225850857650003E-2</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1755,10 +1746,10 @@
         <v>5</v>
       </c>
       <c r="F56">
-        <v>0.39046391752577297</v>
+        <v>0.24140893470790301</v>
       </c>
       <c r="G56">
-        <v>6.5110565110565094E-2</v>
+        <v>5.1549755301794398E-2</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -3167,10 +3158,10 @@
         <v>1</v>
       </c>
       <c r="F117">
-        <v>0.115794653108085</v>
+        <v>0.118090864359521</v>
       </c>
       <c r="G117">
-        <v>0.10028916198632</v>
+        <v>3.3531668798309398E-2</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3190,7 +3181,7 @@
         <v>2</v>
       </c>
       <c r="F118">
-        <v>0.10595374774479201</v>
+        <v>0.10823220728107499</v>
       </c>
       <c r="G118">
         <v>0.21726074626035699</v>
@@ -3213,10 +3204,10 @@
         <v>3</v>
       </c>
       <c r="F119">
-        <v>0.107757913728062</v>
+        <v>0.107740242702525</v>
       </c>
       <c r="G119">
-        <v>0.14244008229994901</v>
+        <v>0.22816145281017999</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3236,10 +3227,10 @@
         <v>4</v>
       </c>
       <c r="F120">
-        <v>0.107593898638674</v>
+        <v>0.119547392587733</v>
       </c>
       <c r="G120">
-        <v>0.22546293721848401</v>
+        <v>7.2655007949125605E-2</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3259,10 +3250,10 @@
         <v>5</v>
       </c>
       <c r="F121">
-        <v>0.109562079711333</v>
+        <v>0.110054124979498</v>
       </c>
       <c r="G121">
-        <v>0.135683701273424</v>
+        <v>0.24330042313117001</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3282,10 +3273,10 @@
         <v>1</v>
       </c>
       <c r="F122">
-        <v>0.116122683286862</v>
+        <v>0.115958668197474</v>
       </c>
       <c r="G122">
-        <v>0.10437635544681</v>
+        <v>8.1243396541177695E-2</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -3305,10 +3296,10 @@
         <v>2</v>
       </c>
       <c r="F123">
-        <v>0.10644579301295699</v>
+        <v>0.104788455231223</v>
       </c>
       <c r="G123">
-        <v>0.20772396151921199</v>
+        <v>0.17420474262579499</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3328,10 +3319,10 @@
         <v>3</v>
       </c>
       <c r="F124">
-        <v>0.107757913728062</v>
+        <v>0.107740242702525</v>
       </c>
       <c r="G124">
-        <v>0.14244008229994901</v>
+        <v>0.22816145281017999</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3351,10 +3342,10 @@
         <v>4</v>
       </c>
       <c r="F125">
-        <v>0.107593898638674</v>
+        <v>0.108724171859626</v>
       </c>
       <c r="G125">
-        <v>0.22546293721848401</v>
+        <v>5.1192368839427599E-2</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3374,21 +3365,21 @@
         <v>5</v>
       </c>
       <c r="F126">
-        <v>0.109562079711333</v>
+        <v>0.110054124979498</v>
       </c>
       <c r="G126">
-        <v>0.135683701273424</v>
+        <v>0.24330042313117001</v>
       </c>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -3397,21 +3388,21 @@
         <v>1</v>
       </c>
       <c r="F127">
-        <v>0.17280453257790299</v>
+        <v>0.28111587982832598</v>
       </c>
       <c r="G127">
-        <v>0.18289664105999401</v>
+        <v>1.30738615327656E-2</v>
       </c>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C128" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -3420,21 +3411,21 @@
         <v>2</v>
       </c>
       <c r="F128">
-        <v>0.1615</v>
+        <v>0.27737226277372201</v>
       </c>
       <c r="G128">
-        <v>0.15326492542313599</v>
+        <v>3.4912376779846599E-2</v>
       </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -3443,21 +3434,21 @@
         <v>3</v>
       </c>
       <c r="F129">
-        <v>0.163833333333333</v>
+        <v>0.341348218119364</v>
       </c>
       <c r="G129">
-        <v>0.16930320932892501</v>
+        <v>2.2655069245242299E-2</v>
       </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B130" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C130" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -3466,21 +3457,21 @@
         <v>4</v>
       </c>
       <c r="F130">
-        <v>0.19516666666666599</v>
+        <v>0.283812795191069</v>
       </c>
       <c r="G130">
-        <v>0.23883980577143299</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="124.2">
+        <v>9.998369831005769E-4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B131" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -3489,24 +3480,22 @@
         <v>5</v>
       </c>
       <c r="F131">
-        <v>0.22837139523253799</v>
+        <v>0.28135738831615098</v>
       </c>
       <c r="G131">
-        <v>5.5760221951340103E-2</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>1.28303425774877E-2</v>
+      </c>
+      <c r="H131" s="1"/>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D132">
         <v>0.1</v>
@@ -3515,21 +3504,21 @@
         <v>1</v>
       </c>
       <c r="F132">
-        <v>0.17913681053157801</v>
+        <v>0.26523605150214502</v>
       </c>
       <c r="G132">
-        <v>0.29520527079048198</v>
+        <v>1.04458666102502E-3</v>
       </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B133" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D133">
         <v>0.1</v>
@@ -3538,21 +3527,21 @@
         <v>2</v>
       </c>
       <c r="F133">
-        <v>0.17249999999999999</v>
+        <v>0.31558608844997799</v>
       </c>
       <c r="G133">
-        <v>0.14860074630939399</v>
+        <v>6.6069472695978598E-2</v>
       </c>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C134" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D134">
         <v>0.1</v>
@@ -3561,21 +3550,21 @@
         <v>3</v>
       </c>
       <c r="F134">
-        <v>0.16816666666666599</v>
+        <v>0.35895234006011101</v>
       </c>
       <c r="G134">
-        <v>0.246210400257701</v>
+        <v>4.5772801579223303E-2</v>
       </c>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B135" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D135">
         <v>0.1</v>
@@ -3584,21 +3573,21 @@
         <v>4</v>
       </c>
       <c r="F135">
-        <v>0.167833333333333</v>
+        <v>0.31386861313868603</v>
       </c>
       <c r="G135">
-        <v>0.279690328161807</v>
+        <v>3.9124055860457699E-3</v>
       </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C136" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D136">
         <v>0.1</v>
@@ -3606,16 +3595,22 @@
       <c r="E136">
         <v>5</v>
       </c>
+      <c r="F136">
+        <v>0.32731958762886598</v>
+      </c>
+      <c r="G136">
+        <v>4.1957585644371902E-2</v>
+      </c>
     </row>
     <row r="137" spans="1:8">
       <c r="A137" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C137" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D137">
         <v>0.01</v>
@@ -3623,16 +3618,25 @@
       <c r="E137">
         <v>1</v>
       </c>
+      <c r="F137">
+        <v>0.30944206008583602</v>
+      </c>
+      <c r="G137">
+        <v>8.7239514465541901E-2</v>
+      </c>
+      <c r="H137" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="138" spans="1:8">
       <c r="A138" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D138">
         <v>0.01</v>
@@ -3640,16 +3644,22 @@
       <c r="E138">
         <v>2</v>
       </c>
+      <c r="F138">
+        <v>0.31472735079433201</v>
+      </c>
+      <c r="G138">
+        <v>0.213229541542794</v>
+      </c>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B139" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C139" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D139">
         <v>0.01</v>
@@ -3657,16 +3667,22 @@
       <c r="E139">
         <v>3</v>
       </c>
+      <c r="F139">
+        <v>0.377415199656504</v>
+      </c>
+      <c r="G139">
+        <v>0.11676845254618901</v>
+      </c>
     </row>
     <row r="140" spans="1:8">
       <c r="A140" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C140" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D140">
         <v>0.01</v>
@@ -3674,22 +3690,264 @@
       <c r="E140">
         <v>4</v>
       </c>
+      <c r="F140">
+        <v>0.31730356376127</v>
+      </c>
+      <c r="G140">
+        <v>0.13081562788675699</v>
+      </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C141" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D141">
         <v>0.01</v>
       </c>
       <c r="E141">
         <v>5</v>
+      </c>
+      <c r="F141">
+        <v>0.32860824742268002</v>
+      </c>
+      <c r="G141">
+        <v>0.19611745513866199</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142" t="s">
+        <v>11</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>0.268669527896995</v>
+      </c>
+      <c r="G142">
+        <v>1.8842227746340701E-4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>15</v>
+      </c>
+      <c r="B143" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="F143">
+        <v>0.247745813653928</v>
+      </c>
+      <c r="G143">
+        <v>7.20935690815208E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>15</v>
+      </c>
+      <c r="B144" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>3</v>
+      </c>
+      <c r="F144">
+        <v>0.33018462859596298</v>
+      </c>
+      <c r="G144">
+        <v>1.68332253786126E-2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" t="s">
+        <v>15</v>
+      </c>
+      <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>4</v>
+      </c>
+      <c r="F145">
+        <v>0.26492056676685199</v>
+      </c>
+      <c r="G145">
+        <v>3.7627922983571503E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>15</v>
+      </c>
+      <c r="B146" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" t="s">
+        <v>8</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>5</v>
+      </c>
+      <c r="F146">
+        <v>0.23840206185567001</v>
+      </c>
+      <c r="G146">
+        <v>3.2030995106035902E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>16</v>
+      </c>
+      <c r="B147" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" t="s">
+        <v>8</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147">
+        <v>0.27939914163090102</v>
+      </c>
+      <c r="G147">
+        <v>7.0311260379753897E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>16</v>
+      </c>
+      <c r="B148" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" t="s">
+        <v>8</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
+      </c>
+      <c r="F148">
+        <v>0.25719192786603601</v>
+      </c>
+      <c r="G148">
+        <v>4.7482136337557899E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>16</v>
+      </c>
+      <c r="B149" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>3</v>
+      </c>
+      <c r="F149">
+        <v>0.31816230141691698</v>
+      </c>
+      <c r="G149">
+        <v>4.4724098578086097E-4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>16</v>
+      </c>
+      <c r="B150" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>4</v>
+      </c>
+      <c r="F150">
+        <v>0.270502361528553</v>
+      </c>
+      <c r="G150">
+        <v>1.2823996087594301E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" t="s">
+        <v>16</v>
+      </c>
+      <c r="B151" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>5</v>
+      </c>
+      <c r="F151">
+        <v>0.24785223367697501</v>
+      </c>
+      <c r="G151">
+        <v>2.3800978792822201E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>